<commit_message>
features significance for big cities & mun
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-6.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-6.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>popsize</t>
   </si>
@@ -75,16 +75,25 @@
     <t>funds</t>
   </si>
   <si>
-    <t>small cities</t>
-  </si>
-  <si>
-    <t>big cities</t>
-  </si>
-  <si>
-    <t>superdataset-31 (big cities only (no mun))</t>
-  </si>
-  <si>
-    <t>superdataset-21 (small cities &amp; muns)</t>
+    <t>superdataset-21 (small cities &amp; muns) 9127 examples</t>
+  </si>
+  <si>
+    <t>superdataset-31 (big cities only (no mun)) 894 examples</t>
+  </si>
+  <si>
+    <t>абс. отклонение</t>
+  </si>
+  <si>
+    <t>значимость (малые)</t>
+  </si>
+  <si>
+    <t>значимость (большие)</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Большая значимость</t>
   </si>
 </sst>
 </file>
@@ -121,12 +130,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -141,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,6 +168,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -433,228 +463,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I21"/>
+  <dimension ref="A2:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>8.876179897426599E-2</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="3">
-        <v>5.6300326620635693E-2</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
+        <v>8.876179897426599E-2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3.837373980721076E-2</v>
+      </c>
+      <c r="G6" s="5">
+        <f>ABS(E6-F6)</f>
+        <v>5.038805916705523E-2</v>
+      </c>
+      <c r="H6" s="7">
+        <f>(E6/F6-1) * 100</f>
+        <v>131.30870074223745</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <f>IF(E6&gt;F6,"small","big")</f>
+        <v>small</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
-        <v>7.0006853020765938E-2</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
+        <v>5.6300326620635693E-2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2.096378317339961E-2</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" ref="G7:G22" si="0">ABS(E7-F7)</f>
+        <v>3.533654344723608E-2</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" ref="H7:H9" si="1">(E7/F7-1) * 100</f>
+        <v>168.559954827589</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <f t="shared" ref="I7:I22" si="2">IF(E7&gt;F7,"small","big")</f>
+        <v>small</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" s="3">
-        <v>4.5450168020463241E-2</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
+        <v>7.0006853020765938E-2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4.1449132236875783E-2</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>2.8557720783890156E-2</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="1"/>
+        <v>68.898235602827398</v>
+      </c>
+      <c r="I8" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>small</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="3">
-        <v>3.7044299736135163E-2</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
+        <v>4.5450168020463241E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>6.2342918491801187E-2</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>1.6892750471337946E-2</v>
+      </c>
+      <c r="H9" s="6">
+        <f>(F9/E9-1) * 100</f>
+        <v>37.167630411690112</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>big</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" s="3">
-        <v>9.6484475997449567E-2</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
+        <v>3.7044299736135163E-2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.19169752921593389</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.15465322947979873</v>
+      </c>
+      <c r="H10" s="7">
+        <f>(F10/E10-1) * 100</f>
+        <v>417.48185437810008</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>big</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="3">
-        <v>7.6727852485608483E-2</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
+        <v>9.6484475997449567E-2</v>
+      </c>
+      <c r="F11" s="3">
+        <v>7.6674481558613644E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
+        <v>1.9809994438835923E-2</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" ref="H11:H17" si="3">(E11/F11-1) * 100</f>
+        <v>25.836489580555178</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>small</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="3">
-        <v>5.1095555697749387E-2</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
+        <v>7.6727852485608483E-2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>6.8816774255497329E-2</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="0"/>
+        <v>7.9110782301111543E-3</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="3"/>
+        <v>11.495857391890452</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>small</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="3">
-        <v>4.7555291053109093E-2</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
+        <v>5.1095555697749387E-2</v>
+      </c>
+      <c r="F13" s="3">
+        <v>4.5818646640167673E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="0"/>
+        <v>5.2769090575817135E-3</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" si="3"/>
+        <v>11.516946580774</v>
+      </c>
+      <c r="I13" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>small</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="3">
-        <v>6.3637719097056025E-2</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="3"/>
+        <v>4.7555291053109093E-2</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4.2393556631766992E-2</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="0"/>
+        <v>5.1617344213421013E-3</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="3"/>
+        <v>12.175752240316239</v>
+      </c>
+      <c r="I14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>small</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="3">
-        <v>3.8792529469582053E-2</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
+        <v>6.3637719097056025E-2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2.3094174678966989E-2</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
+        <v>4.0543544418089036E-2</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="3"/>
+        <v>175.55745109615916</v>
+      </c>
+      <c r="I15" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>small</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="3">
-        <v>9.8917956653452391E-2</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
+        <v>3.8792529469582053E-2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>3.2676097925639219E-2</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="0"/>
+        <v>6.1164315439428338E-3</v>
+      </c>
+      <c r="H16" s="8">
+        <f t="shared" si="3"/>
+        <v>18.718365815471461</v>
+      </c>
+      <c r="I16" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>small</v>
+      </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="3">
-        <v>3.5033101077425528E-2</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
+        <v>9.8917956653452391E-2</v>
+      </c>
+      <c r="F17" s="3">
+        <v>4.2422006031541802E-2</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>5.6495950621910589E-2</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="3"/>
+        <v>133.17604683735246</v>
+      </c>
+      <c r="I17" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>small</v>
+      </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E18" s="3">
-        <v>3.3044783845680173E-2</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
+        <v>3.5033101077425528E-2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>5.2552382589893337E-2</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7519281512467809E-2</v>
+      </c>
+      <c r="H18" s="6">
+        <f>(F18/E18-1) * 100</f>
+        <v>50.007795409687006</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>big</v>
+      </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3">
-        <v>4.0489178065095242E-2</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="3"/>
+        <v>3.3044783845680173E-2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.10942389951332911</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="0"/>
+        <v>7.6379115667648934E-2</v>
+      </c>
+      <c r="H19" s="7">
+        <f t="shared" ref="H19:H20" si="4">(F19/E19-1) * 100</f>
+        <v>231.13819120240274</v>
+      </c>
+      <c r="I19" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>big</v>
+      </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="3">
-        <v>5.1037039760890517E-2</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="3"/>
+        <v>4.0489178065095242E-2</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.10095805870141331</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="0"/>
+        <v>6.0468880636318063E-2</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="4"/>
+        <v>149.34578454297358</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>big</v>
+      </c>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="3">
+        <v>5.1037039760890517E-2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2.2808132644413968E-2</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="0"/>
+        <v>2.8228907116476548E-2</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" ref="H21:H22" si="5">(E21/F21-1) * 100</f>
+        <v>123.76684911726082</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>small</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E22" s="3">
         <v>6.9621070424635514E-2</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
+      <c r="F22" s="3">
+        <v>2.753468590353542E-2</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="0"/>
+        <v>4.2086384521100098E-2</v>
+      </c>
+      <c r="H22" s="7">
+        <f t="shared" si="5"/>
+        <v>152.84860945407135</v>
+      </c>
+      <c r="I22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>small</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
features significance for positive flow
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-6.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-6.xlsx
@@ -4,16 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="small vs big (features)" sheetId="1" r:id="rId1"/>
+    <sheet name="positive vs negative &amp; class" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'small vs big (features)'!$D$6:$D$22</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'small vs big (features)'!$E$6:$E$22</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'small vs big (features)'!$F$6:$F$22</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>popsize</t>
   </si>
@@ -100,6 +96,18 @@
   <si>
     <t>Большая значимость для</t>
   </si>
+  <si>
+    <t>superdataset-21 (negative flow).csv - 6510 examples</t>
+  </si>
+  <si>
+    <t>superdataset-21 (positive flow).csv - 1796 examples</t>
+  </si>
+  <si>
+    <t>значимость (приток)</t>
+  </si>
+  <si>
+    <t>значимость (отток)</t>
+  </si>
 </sst>
 </file>
 
@@ -161,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,6 +194,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2734,8 +2745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3178,4 +3189,415 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.19651338695908471</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="10">
+        <f>ABS(G9-H9)</f>
+        <v>0.19651338695908471</v>
+      </c>
+      <c r="J9" s="8" t="e">
+        <f>(G9/H9-1) * 100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="2" t="str">
+        <f>IF(G9&gt;H9,"+","-")</f>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>8.4246437431035742E-2</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="10">
+        <f t="shared" ref="I10:I25" si="0">ABS(G10-H10)</f>
+        <v>8.4246437431035742E-2</v>
+      </c>
+      <c r="J10" s="8" t="e">
+        <f t="shared" ref="J10:J11" si="1">(G10/H10-1) * 100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="2" t="str">
+        <f t="shared" ref="K10:K25" si="2">IF(G10&gt;H10,"+","-")</f>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="3">
+        <v>6.0922716814600333E-2</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="10">
+        <f t="shared" si="0"/>
+        <v>6.0922716814600333E-2</v>
+      </c>
+      <c r="J11" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5.2062335266720473E-2</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="10">
+        <f t="shared" si="0"/>
+        <v>5.2062335266720473E-2</v>
+      </c>
+      <c r="J12" s="8">
+        <f>(H12/G12-1) * 100</f>
+        <v>-100</v>
+      </c>
+      <c r="K12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2.443431828231071E-2</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="10">
+        <f t="shared" si="0"/>
+        <v>2.443431828231071E-2</v>
+      </c>
+      <c r="J13" s="8">
+        <f>(H13/G13-1) * 100</f>
+        <v>-100</v>
+      </c>
+      <c r="K13" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="3">
+        <v>7.6084702155837111E-2</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="10">
+        <f t="shared" si="0"/>
+        <v>7.6084702155837111E-2</v>
+      </c>
+      <c r="J14" s="8" t="e">
+        <f t="shared" ref="J14:J20" si="3">(G14/H14-1) * 100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.111861084259628</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="10">
+        <f t="shared" si="0"/>
+        <v>0.111861084259628</v>
+      </c>
+      <c r="J15" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="3">
+        <v>3.0463837532272241E-2</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="10">
+        <f t="shared" si="0"/>
+        <v>3.0463837532272241E-2</v>
+      </c>
+      <c r="J16" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K16" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2.9962570531213661E-2</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="10">
+        <f t="shared" si="0"/>
+        <v>2.9962570531213661E-2</v>
+      </c>
+      <c r="J17" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="3">
+        <v>5.9938041871093951E-2</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="10">
+        <f t="shared" si="0"/>
+        <v>5.9938041871093951E-2</v>
+      </c>
+      <c r="J18" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2.9289504050935729E-2</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="10">
+        <f t="shared" si="0"/>
+        <v>2.9289504050935729E-2</v>
+      </c>
+      <c r="J19" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="20" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="3">
+        <v>9.1904161425450603E-2</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="10">
+        <f t="shared" si="0"/>
+        <v>9.1904161425450603E-2</v>
+      </c>
+      <c r="J20" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K20" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1.997123759402095E-2</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="10">
+        <f t="shared" si="0"/>
+        <v>1.997123759402095E-2</v>
+      </c>
+      <c r="J21" s="8">
+        <f>(H21/G21-1) * 100</f>
+        <v>-100</v>
+      </c>
+      <c r="K21" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2.9643758880956089E-2</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="10">
+        <f t="shared" si="0"/>
+        <v>2.9643758880956089E-2</v>
+      </c>
+      <c r="J22" s="8">
+        <f t="shared" ref="J22:J23" si="4">(H22/G22-1) * 100</f>
+        <v>-100</v>
+      </c>
+      <c r="K22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="23" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="3">
+        <v>3.0664861454868748E-2</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="10">
+        <f t="shared" si="0"/>
+        <v>3.0664861454868748E-2</v>
+      </c>
+      <c r="J23" s="8">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="K23" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="24" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="3">
+        <v>3.044951080338432E-2</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="10">
+        <f t="shared" si="0"/>
+        <v>3.044951080338432E-2</v>
+      </c>
+      <c r="J24" s="8" t="e">
+        <f t="shared" ref="J24:J25" si="5">(G24/H24-1) * 100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K24" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="25" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="3">
+        <v>4.158753468658663E-2</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="10">
+        <f t="shared" si="0"/>
+        <v>4.158753468658663E-2</v>
+      </c>
+      <c r="J25" s="8" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K25" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
features significance for negative flow
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-6.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-6.xlsx
@@ -143,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +153,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,6 +203,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1291,6 +1306,516 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Приток</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'positive vs negative &amp; class'!$F$9:$F$25</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>popsize</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>avgemployers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>avgsalary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shoparea</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>retailturnover</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>livarea</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>roadslen</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>livestock</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>harvest</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>agrprod</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>funds</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>hospitals</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>beforeschool</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>factoriescap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'positive vs negative &amp; class'!$G$9:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.19651338695908471</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4246437431035742E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0922716814600333E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2062335266720473E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.443431828231071E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.6084702155837111E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.111861084259628</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0463837532272241E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9962570531213661E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.9938041871093951E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.9289504050935729E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.1904161425450603E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.997123759402095E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.9643758880956089E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0664861454868748E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.044951080338432E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.158753468658663E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-020C-4145-91D4-0ED7CDD62037}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Отток</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'positive vs negative &amp; class'!$F$9:$F$25</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>popsize</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>avgemployers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>avgsalary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shoparea</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>retailturnover</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>livarea</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>roadslen</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>livestock</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>harvest</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>agrprod</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>funds</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>hospitals</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>beforeschool</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>factoriescap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'positive vs negative &amp; class'!$H$9:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.26980375759711211</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9000406028132548E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6320219871066464E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6706129254384462E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4108521705298427E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0843845459607781E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4697653471483768E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8148530659469063E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2108360406245137E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0741580288573678E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0174008143912532E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.5306804708399963E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0471539894795502E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.3615198845875752E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.2034046209899622E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.7324435146223974E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.8594962309519247E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-020C-4145-91D4-0ED7CDD62037}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="1863884160"/>
+        <c:axId val="1863886656"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1863884160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1863886656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1863886656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1863884160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1371,6 +1896,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
   <cs:axisTitle>
@@ -2400,6 +2965,525 @@
       <a:schemeClr val="tx1">
         <a:lumMod val="50000"/>
         <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2472,6 +3556,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2746,7 +3865,7 @@
   <dimension ref="A2:I22"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:I22"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3195,8 +4314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3240,44 +4359,48 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="12">
         <v>0.19651338695908471</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="10">
+      <c r="H9" s="12">
+        <v>0.26980375759711211</v>
+      </c>
+      <c r="I9" s="12">
         <f>ABS(G9-H9)</f>
-        <v>0.19651338695908471</v>
-      </c>
-      <c r="J9" s="8" t="e">
-        <f>(G9/H9-1) * 100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K9" s="2" t="str">
+        <v>7.3290370638027402E-2</v>
+      </c>
+      <c r="J9" s="13">
+        <f>(H9/G9-1) * 100</f>
+        <v>37.295357722009491</v>
+      </c>
+      <c r="K9" s="11" t="str">
         <f>IF(G9&gt;H9,"+","-")</f>
-        <v>+</v>
+        <v>-</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="12">
         <v>8.4246437431035742E-2</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="10">
+      <c r="H10" s="12">
+        <v>4.9000406028132548E-2</v>
+      </c>
+      <c r="I10" s="12">
         <f t="shared" ref="I10:I25" si="0">ABS(G10-H10)</f>
-        <v>8.4246437431035742E-2</v>
-      </c>
-      <c r="J10" s="8" t="e">
-        <f t="shared" ref="J10:J11" si="1">(G10/H10-1) * 100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K10" s="2" t="str">
-        <f t="shared" ref="K10:K25" si="2">IF(G10&gt;H10,"+","-")</f>
+        <v>3.5246031402903194E-2</v>
+      </c>
+      <c r="J10" s="13">
+        <f>(G10/H10-1) * 100</f>
+        <v>71.930080299064116</v>
+      </c>
+      <c r="K10" s="11" t="str">
+        <f t="shared" ref="K10:K25" si="1">IF(G10&gt;H10,"+","-")</f>
         <v>+</v>
       </c>
     </row>
@@ -3288,18 +4411,20 @@
       <c r="G11" s="3">
         <v>6.0922716814600333E-2</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3">
+        <v>7.6320219871066464E-2</v>
+      </c>
       <c r="I11" s="10">
         <f t="shared" si="0"/>
-        <v>6.0922716814600333E-2</v>
-      </c>
-      <c r="J11" s="8" t="e">
+        <v>1.539750305646613E-2</v>
+      </c>
+      <c r="J11" s="8">
+        <f>(H11/G11-1) * 100</f>
+        <v>25.2738286497034</v>
+      </c>
+      <c r="K11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K11" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>+</v>
+        <v>-</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3309,17 +4434,19 @@
       <c r="G12" s="3">
         <v>5.2062335266720473E-2</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3">
+        <v>3.6706129254384462E-2</v>
+      </c>
       <c r="I12" s="10">
         <f t="shared" si="0"/>
-        <v>5.2062335266720473E-2</v>
+        <v>1.5356206012336011E-2</v>
       </c>
       <c r="J12" s="8">
-        <f>(H12/G12-1) * 100</f>
-        <v>-100</v>
+        <f t="shared" ref="J12" si="2">(G12/H12-1) * 100</f>
+        <v>41.83553625584684</v>
       </c>
       <c r="K12" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>+</v>
       </c>
     </row>
@@ -3330,18 +4457,20 @@
       <c r="G13" s="3">
         <v>2.443431828231071E-2</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3">
+        <v>3.4108521705298427E-2</v>
+      </c>
       <c r="I13" s="10">
         <f t="shared" si="0"/>
-        <v>2.443431828231071E-2</v>
+        <v>9.674203422987717E-3</v>
       </c>
       <c r="J13" s="8">
         <f>(H13/G13-1) * 100</f>
-        <v>-100</v>
+        <v>39.592688084084514</v>
       </c>
       <c r="K13" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>+</v>
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3351,38 +4480,42 @@
       <c r="G14" s="3">
         <v>7.6084702155837111E-2</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="3">
+        <v>5.0843845459607781E-2</v>
+      </c>
       <c r="I14" s="10">
         <f t="shared" si="0"/>
-        <v>7.6084702155837111E-2</v>
-      </c>
-      <c r="J14" s="8" t="e">
-        <f t="shared" ref="J14:J20" si="3">(G14/H14-1) * 100</f>
-        <v>#DIV/0!</v>
+        <v>2.524085669622933E-2</v>
+      </c>
+      <c r="J14" s="8">
+        <f t="shared" ref="J14:J15" si="3">(G14/H14-1) * 100</f>
+        <v>49.643878168659761</v>
       </c>
       <c r="K14" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>+</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="12">
         <v>0.111861084259628</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="10">
+      <c r="H15" s="12">
+        <v>5.4697653471483768E-2</v>
+      </c>
+      <c r="I15" s="12">
         <f t="shared" si="0"/>
-        <v>0.111861084259628</v>
-      </c>
-      <c r="J15" s="8" t="e">
+        <v>5.7163430788144232E-2</v>
+      </c>
+      <c r="J15" s="13">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K15" s="2" t="str">
-        <f t="shared" si="2"/>
+        <v>104.50801297709411</v>
+      </c>
+      <c r="K15" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>+</v>
       </c>
     </row>
@@ -3393,18 +4526,20 @@
       <c r="G16" s="3">
         <v>3.0463837532272241E-2</v>
       </c>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3">
+        <v>3.8148530659469063E-2</v>
+      </c>
       <c r="I16" s="10">
         <f t="shared" si="0"/>
-        <v>3.0463837532272241E-2</v>
-      </c>
-      <c r="J16" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>7.6846931271968219E-3</v>
+      </c>
+      <c r="J16" s="8">
+        <f>(H16/G16-1) * 100</f>
+        <v>25.22562405033819</v>
       </c>
       <c r="K16" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>+</v>
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
     </row>
     <row r="17" spans="6:11" x14ac:dyDescent="0.25">
@@ -3414,18 +4549,20 @@
       <c r="G17" s="3">
         <v>2.9962570531213661E-2</v>
       </c>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3">
+        <v>3.2108360406245137E-2</v>
+      </c>
       <c r="I17" s="10">
         <f t="shared" si="0"/>
-        <v>2.9962570531213661E-2</v>
-      </c>
-      <c r="J17" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>2.1457898750314765E-3</v>
+      </c>
+      <c r="J17" s="8">
+        <f>(H17/G17-1) * 100</f>
+        <v>7.1615680396850179</v>
       </c>
       <c r="K17" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>+</v>
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
     </row>
     <row r="18" spans="6:11" x14ac:dyDescent="0.25">
@@ -3435,17 +4572,19 @@
       <c r="G18" s="3">
         <v>5.9938041871093951E-2</v>
       </c>
-      <c r="H18" s="3"/>
+      <c r="H18" s="3">
+        <v>4.0741580288573678E-2</v>
+      </c>
       <c r="I18" s="10">
         <f t="shared" si="0"/>
-        <v>5.9938041871093951E-2</v>
-      </c>
-      <c r="J18" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.9196461582520273E-2</v>
+      </c>
+      <c r="J18" s="8">
+        <f t="shared" ref="J18" si="4">(G18/H18-1) * 100</f>
+        <v>47.117616564088173</v>
       </c>
       <c r="K18" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>+</v>
       </c>
     </row>
@@ -3456,60 +4595,66 @@
       <c r="G19" s="3">
         <v>2.9289504050935729E-2</v>
       </c>
-      <c r="H19" s="3"/>
+      <c r="H19" s="3">
+        <v>4.0174008143912532E-2</v>
+      </c>
       <c r="I19" s="10">
         <f t="shared" si="0"/>
-        <v>2.9289504050935729E-2</v>
-      </c>
-      <c r="J19" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.0884504092976803E-2</v>
+      </c>
+      <c r="J19" s="8">
+        <f>(H19/G19-1) * 100</f>
+        <v>37.161790360288016</v>
       </c>
       <c r="K19" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>+</v>
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
     </row>
     <row r="20" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="12">
         <v>9.1904161425450603E-2</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="10">
+      <c r="H20" s="12">
+        <v>4.5306804708399963E-2</v>
+      </c>
+      <c r="I20" s="12">
         <f t="shared" si="0"/>
-        <v>9.1904161425450603E-2</v>
-      </c>
-      <c r="J20" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" s="2" t="str">
-        <f t="shared" si="2"/>
+        <v>4.6597356717050641E-2</v>
+      </c>
+      <c r="J20" s="13">
+        <f t="shared" ref="J20" si="5">(G20/H20-1) * 100</f>
+        <v>102.84847279996198</v>
+      </c>
+      <c r="K20" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>+</v>
       </c>
     </row>
     <row r="21" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="12">
         <v>1.997123759402095E-2</v>
       </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="10">
+      <c r="H21" s="12">
+        <v>4.0471539894795502E-2</v>
+      </c>
+      <c r="I21" s="12">
         <f t="shared" si="0"/>
-        <v>1.997123759402095E-2</v>
-      </c>
-      <c r="J21" s="8">
+        <v>2.0500302300774553E-2</v>
+      </c>
+      <c r="J21" s="13">
         <f>(H21/G21-1) * 100</f>
-        <v>-100</v>
-      </c>
-      <c r="K21" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>+</v>
+        <v>102.64913330615019</v>
+      </c>
+      <c r="K21" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
     </row>
     <row r="22" spans="6:11" x14ac:dyDescent="0.25">
@@ -3519,18 +4664,20 @@
       <c r="G22" s="3">
         <v>2.9643758880956089E-2</v>
       </c>
-      <c r="H22" s="3"/>
+      <c r="H22" s="3">
+        <v>4.3615198845875752E-2</v>
+      </c>
       <c r="I22" s="10">
         <f t="shared" si="0"/>
-        <v>2.9643758880956089E-2</v>
+        <v>1.3971439964919664E-2</v>
       </c>
       <c r="J22" s="8">
-        <f t="shared" ref="J22:J23" si="4">(H22/G22-1) * 100</f>
-        <v>-100</v>
+        <f t="shared" ref="J22:J24" si="6">(H22/G22-1) * 100</f>
+        <v>47.131134823442643</v>
       </c>
       <c r="K22" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>+</v>
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
     </row>
     <row r="23" spans="6:11" x14ac:dyDescent="0.25">
@@ -3540,39 +4687,43 @@
       <c r="G23" s="3">
         <v>3.0664861454868748E-2</v>
       </c>
-      <c r="H23" s="3"/>
+      <c r="H23" s="3">
+        <v>3.2034046209899622E-2</v>
+      </c>
       <c r="I23" s="10">
         <f t="shared" si="0"/>
-        <v>3.0664861454868748E-2</v>
+        <v>1.3691847550308736E-3</v>
       </c>
       <c r="J23" s="8">
-        <f t="shared" si="4"/>
-        <v>-100</v>
+        <f t="shared" si="6"/>
+        <v>4.4649957315019417</v>
       </c>
       <c r="K23" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>+</v>
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
     </row>
     <row r="24" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="12">
         <v>3.044951080338432E-2</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="10">
+      <c r="H24" s="12">
+        <v>7.7324435146223974E-2</v>
+      </c>
+      <c r="I24" s="12">
         <f t="shared" si="0"/>
-        <v>3.044951080338432E-2</v>
-      </c>
-      <c r="J24" s="8" t="e">
-        <f t="shared" ref="J24:J25" si="5">(G24/H24-1) * 100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K24" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>+</v>
+        <v>4.6874924342839658E-2</v>
+      </c>
+      <c r="J24" s="13">
+        <f t="shared" si="6"/>
+        <v>153.94311141980555</v>
+      </c>
+      <c r="K24" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
     </row>
     <row r="25" spans="6:11" x14ac:dyDescent="0.25">
@@ -3582,22 +4733,25 @@
       <c r="G25" s="3">
         <v>4.158753468658663E-2</v>
       </c>
-      <c r="H25" s="3"/>
+      <c r="H25" s="3">
+        <v>3.8594962309519247E-2</v>
+      </c>
       <c r="I25" s="10">
         <f t="shared" si="0"/>
-        <v>4.158753468658663E-2</v>
-      </c>
-      <c r="J25" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>2.9925723770673832E-3</v>
+      </c>
+      <c r="J25" s="8">
+        <f t="shared" ref="J24:J25" si="7">(G25/H25-1) * 100</f>
+        <v>7.7537901269805865</v>
       </c>
       <c r="K25" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>+</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
features significance for classifier
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-6.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-6.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="small vs big (features)" sheetId="1" r:id="rId1"/>
-    <sheet name="positive vs negative &amp; class" sheetId="2" r:id="rId2"/>
+    <sheet name="positive vs negative" sheetId="2" r:id="rId2"/>
+    <sheet name="classifier" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'positive vs negative &amp; class'!$F$9:$F$25</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'positive vs negative &amp; class'!$G$9:$G$25</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'positive vs negative &amp; class'!$H$9:$H$25</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">classifier!$D$8:$D$24</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">classifier!$E$8:$E$24</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
   <si>
     <t>popsize</t>
   </si>
@@ -113,6 +113,9 @@
   <si>
     <t>значимость (отток)</t>
   </si>
+  <si>
+    <t>значимость (класс)</t>
+  </si>
 </sst>
 </file>
 
@@ -180,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -220,6 +223,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1365,7 +1377,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'positive vs negative &amp; class'!$F$9:$F$25</c:f>
+              <c:f>'positive vs negative'!$F$9:$F$25</c:f>
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
@@ -1424,7 +1436,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'positive vs negative &amp; class'!$G$9:$G$25</c:f>
+              <c:f>'positive vs negative'!$G$9:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1518,7 +1530,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'positive vs negative &amp; class'!$F$9:$F$25</c:f>
+              <c:f>'positive vs negative'!$F$9:$F$25</c:f>
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
@@ -1577,7 +1589,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'positive vs negative &amp; class'!$H$9:$H$25</c:f>
+              <c:f>'positive vs negative'!$H$9:$H$25</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1864,7 +1876,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'positive vs negative &amp; class'!$F$9:$F$25</c:f>
+              <c:f>'positive vs negative'!$F$9:$F$25</c:f>
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
@@ -1923,7 +1935,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'positive vs negative &amp; class'!$G$9:$G$25</c:f>
+              <c:f>'positive vs negative'!$G$9:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2007,7 +2019,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'positive vs negative &amp; class'!$F$9:$F$25</c:f>
+              <c:f>'positive vs negative'!$F$9:$F$25</c:f>
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
@@ -2066,7 +2078,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'positive vs negative &amp; class'!$H$9:$H$25</c:f>
+              <c:f>'positive vs negative'!$H$9:$H$25</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2325,6 +2337,417 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU" b="0"/>
+              <a:t>Классификатор</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" b="0" baseline="0"/>
+              <a:t> (отток/приток)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>classifier!$D$8:$D$24</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>popsize</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>avgemployers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>avgsalary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shoparea</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>retailturnover</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>livarea</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>roadslen</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>livestock</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>harvest</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>agrprod</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>funds</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>hospitals</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>beforeschool</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>factoriescap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>classifier!$E$8:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>3.023124929965313E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4946025414946776E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18458519067240159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5643273327995392E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0353447973308759E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3371201925933873E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.54661209470425964</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5025530416919998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9016226211152681E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.294752092163343E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1265382058683148</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.1999575141071673E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.154940258842845E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1374393633140171E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.538769185365546E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.4383027215276162E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.9108485122103564E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-42A0-4A4E-B83B-E76D3AAC6008}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="633524975"/>
+        <c:axId val="633527055"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="633524975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="633527055"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="633527055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="633524975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2485,6 +2908,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
   <cs:axisTitle>
@@ -4050,6 +4513,531 @@
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="206">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="219">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4703,6 +5691,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1019174</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>157161</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
@@ -4969,7 +5992,7 @@
   <dimension ref="A2:I22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5418,8 +6441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5858,4 +6881,246 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D5:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3.023124929965313E-3</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
+        <v>8.4946025414946776E-3</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.18458519067240159</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2.5643273327995392E-3</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="8">
+        <v>3.0353447973308759E-2</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="8">
+        <v>5.3371201925933873E-3</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.54661209470425964</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="8">
+        <v>3.5025530416919998E-2</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="8">
+        <v>2.9016226211152681E-3</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1.294752092163343E-2</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.1265382058683148</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="8">
+        <v>5.1999575141071673E-3</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="8">
+        <v>9.154940258842845E-3</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1.1374393633140171E-2</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="8">
+        <v>3.538769185365546E-3</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="8">
+        <v>7.4383027215276162E-3</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="8">
+        <v>4.9108485122103564E-3</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>